<commit_message>
Added wrangle function and tests for 3 or more columns
</commit_message>
<xml_diff>
--- a/inst/extdata/Fake3Columns.xlsx
+++ b/inst/extdata/Fake3Columns.xlsx
@@ -1,52 +1,71 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sharon\My Documents Data Drive\R\elections2\inst\extdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A49FA65-16CD-4C54-9DD7-24B3E42F9128}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="8925" yWindow="1920" windowWidth="17160" windowHeight="13410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t xml:space="preserve">City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City C</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>City A</t>
+  </si>
+  <si>
+    <t>City B</t>
+  </si>
+  <si>
+    <t>City C</t>
+  </si>
+  <si>
+    <t>City D</t>
+  </si>
+  <si>
+    <t>City E</t>
+  </si>
+  <si>
+    <t>City Ties</t>
+  </si>
+  <si>
+    <t>City F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -82,6 +101,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -363,14 +391,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -390,68 +420,148 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>2698</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>229</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>982</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>771</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>309</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>407</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>562</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>212</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>562</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>303</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>300</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>297</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>250</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>297</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>1023</v>
+      </c>
+      <c r="C5">
+        <v>2025</v>
+      </c>
+      <c r="D5">
+        <v>400</v>
+      </c>
+      <c r="E5">
+        <v>1034</v>
+      </c>
+      <c r="F5">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>1600</v>
+      </c>
+      <c r="C6">
+        <v>1800</v>
+      </c>
+      <c r="D6">
+        <v>1700</v>
+      </c>
+      <c r="E6">
+        <v>1700</v>
+      </c>
+      <c r="F6">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>300</v>
+      </c>
+      <c r="C7">
+        <v>400</v>
+      </c>
+      <c r="D7">
+        <v>300</v>
+      </c>
+      <c r="E7">
+        <v>400</v>
+      </c>
+      <c r="F7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>456</v>
+      </c>
+      <c r="C8">
+        <v>723</v>
+      </c>
+      <c r="D8">
+        <v>244</v>
+      </c>
+      <c r="E8">
+        <v>500</v>
+      </c>
+      <c r="F8">
+        <v>456</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed errors when there's missing data
</commit_message>
<xml_diff>
--- a/inst/extdata/Fake3Columns.xlsx
+++ b/inst/extdata/Fake3Columns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sharon\My Documents Data Drive\R\elections2\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A49FA65-16CD-4C54-9DD7-24B3E42F9128}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F919A727-8AEE-4621-8E96-F9A9B420FAFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8925" yWindow="1920" windowWidth="17160" windowHeight="13410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>City</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>City F</t>
+  </si>
+  <si>
+    <t>City Z</t>
   </si>
 </sst>
 </file>
@@ -392,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,81 +485,86 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>1023</v>
-      </c>
-      <c r="C5">
-        <v>2025</v>
-      </c>
-      <c r="D5">
-        <v>400</v>
-      </c>
-      <c r="E5">
-        <v>1034</v>
-      </c>
-      <c r="F5">
-        <v>505</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>1600</v>
+        <v>1023</v>
       </c>
       <c r="C6">
-        <v>1800</v>
+        <v>2025</v>
       </c>
       <c r="D6">
-        <v>1700</v>
+        <v>400</v>
       </c>
       <c r="E6">
-        <v>1700</v>
+        <v>1034</v>
       </c>
       <c r="F6">
-        <v>1609</v>
+        <v>505</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>300</v>
+        <v>1600</v>
       </c>
       <c r="C7">
-        <v>400</v>
+        <v>1800</v>
       </c>
       <c r="D7">
-        <v>300</v>
+        <v>1700</v>
       </c>
       <c r="E7">
-        <v>400</v>
+        <v>1700</v>
       </c>
       <c r="F7">
-        <v>400</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>300</v>
+      </c>
+      <c r="C8">
+        <v>400</v>
+      </c>
+      <c r="D8">
+        <v>300</v>
+      </c>
+      <c r="E8">
+        <v>400</v>
+      </c>
+      <c r="F8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>456</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>723</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>244</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>500</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>456</v>
       </c>
     </row>

</xml_diff>